<commit_message>
Segment Tree and Binary Indexed Tree Added
</commit_message>
<xml_diff>
--- a/Problems.xlsx
+++ b/Problems.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selman/Google Drive/Master/First Year/First semester/Competitive programming and contests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selman/Google Drive/Master/First Year/First semester/Competitive programming and contests/Github/CompetitiveProgramming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D94572-8E3B-664D-81E1-974656C1D394}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701A333A-F393-A549-94FE-994359B27E0D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{59DA6F5E-AF74-844C-9459-D868A740F883}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{59DA6F5E-AF74-844C-9459-D868A740F883}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
   <si>
     <t>Problem</t>
   </si>
@@ -144,9 +144,6 @@
     <t xml:space="preserve">O(n) with Dequeu </t>
   </si>
   <si>
-    <t>Data Structure or Algorithm</t>
-  </si>
-  <si>
     <t>Dequeu</t>
   </si>
   <si>
@@ -160,6 +157,12 @@
   </si>
   <si>
     <t>Stack</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Structure </t>
   </si>
 </sst>
 </file>
@@ -295,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -320,20 +323,64 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
+        <color rgb="FFFF0000"/>
         <name val="Times New Roman"/>
         <family val="1"/>
         <scheme val="none"/>
@@ -345,7 +392,75 @@
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -380,6 +495,72 @@
         <left style="thin">
           <color auto="1"/>
         </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -418,141 +599,6 @@
         <right style="thin">
           <color auto="1"/>
         </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -621,14 +667,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>1053821</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>99004</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="180627" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -670,6 +716,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -709,7 +756,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -781,8 +828,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D938C518-70BF-5A4D-B2E3-CBDA392058BE}" name="Table2" displayName="Table2" ref="A1:G27" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G27" xr:uid="{591EFFBC-CF6E-4749-B9B1-AA3DBEFC5570}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D938C518-70BF-5A4D-B2E3-CBDA392058BE}" name="Table2" displayName="Table2" ref="A1:H27" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H27" xr:uid="{591EFFBC-CF6E-4749-B9B1-AA3DBEFC5570}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -790,15 +837,17 @@
     <filterColumn colId="4" hiddenButton="1"/>
     <filterColumn colId="5" hiddenButton="1"/>
     <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{ACAC2441-A820-944F-9AF2-3F5E4FB31EA0}" name="Problem" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{D488543C-E183-BF44-8C30-17372FA97B14}" name="Data Structure or Algorithm" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{44ECDE62-26AB-614D-9A95-A825F8E84A50}" name="Progress" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{4426360F-515C-E249-8E56-5FFEBDF610C5}" name="Explanation" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{BDCE3B2A-F2CA-7940-A777-18C5FE8F8250}" name=" Best Complexity" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{6F0E44E4-9DBC-9E41-B548-48FF281C4DE7}" name="Optimal Complexity" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{4E2B027C-84E2-4746-A050-99003D6F130D}" name=" Brute Force Complexity" dataDxfId="5"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{ACAC2441-A820-944F-9AF2-3F5E4FB31EA0}" name="Problem" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{FBEAA6B8-E7D6-F748-9496-1911EE208A06}" name="Algorithm" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{D488543C-E183-BF44-8C30-17372FA97B14}" name="Data Structure " dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{44ECDE62-26AB-614D-9A95-A825F8E84A50}" name="Progress" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{4426360F-515C-E249-8E56-5FFEBDF610C5}" name="Explanation" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{BDCE3B2A-F2CA-7940-A777-18C5FE8F8250}" name=" Best Complexity" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{6F0E44E4-9DBC-9E41-B548-48FF281C4DE7}" name="Optimal Complexity" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{4E2B027C-84E2-4746-A050-99003D6F130D}" name=" Brute Force Complexity" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1101,470 +1150,500 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E486DD-8F02-B64F-98E1-BE648EE83720}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F26" sqref="F2:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13" style="2" customWidth="1"/>
-    <col min="5" max="5" width="26" style="2" customWidth="1"/>
-    <col min="6" max="6" width="38.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.1640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="11" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26" style="2" customWidth="1"/>
+    <col min="7" max="7" width="38.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="14"/>
       <c r="D3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" s="6"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>30</v>
+      <c r="B7" s="9"/>
+      <c r="C7" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" s="6"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="6" t="s">
+      <c r="E9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="11" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="14"/>
       <c r="D16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E19" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="14"/>
       <c r="D20" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E21" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E22" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E23" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E24" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E25" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="14"/>
       <c r="D26" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E26" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="8"/>
+      <c r="E27" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Longest Decreasing/Increasing Subsequence Added
</commit_message>
<xml_diff>
--- a/Problems.xlsx
+++ b/Problems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selman/Google Drive/Master/First Year/First semester/Competitive programming and contests/Github/CompetitiveProgramming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701A333A-F393-A549-94FE-994359B27E0D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FA38F3-953B-6145-A53B-4E8BBC812FB7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{59DA6F5E-AF74-844C-9459-D868A740F883}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{59DA6F5E-AF74-844C-9459-D868A740F883}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
   <si>
     <t>Problem</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t xml:space="preserve">Data Structure </t>
+  </si>
+  <si>
+    <t>Longest Increasing Subsequence</t>
+  </si>
+  <si>
+    <t>Longest Decreasing Subsequence</t>
   </si>
 </sst>
 </file>
@@ -245,7 +251,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -294,11 +300,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -326,11 +354,219 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -369,207 +605,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -828,8 +863,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D938C518-70BF-5A4D-B2E3-CBDA392058BE}" name="Table2" displayName="Table2" ref="A1:H27" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H27" xr:uid="{591EFFBC-CF6E-4749-B9B1-AA3DBEFC5570}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D938C518-70BF-5A4D-B2E3-CBDA392058BE}" name="Table2" displayName="Table2" ref="A1:H30" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H30" xr:uid="{591EFFBC-CF6E-4749-B9B1-AA3DBEFC5570}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -841,13 +876,13 @@
   </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{ACAC2441-A820-944F-9AF2-3F5E4FB31EA0}" name="Problem" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{FBEAA6B8-E7D6-F748-9496-1911EE208A06}" name="Algorithm" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{D488543C-E183-BF44-8C30-17372FA97B14}" name="Data Structure " dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{44ECDE62-26AB-614D-9A95-A825F8E84A50}" name="Progress" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{4426360F-515C-E249-8E56-5FFEBDF610C5}" name="Explanation" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{BDCE3B2A-F2CA-7940-A777-18C5FE8F8250}" name=" Best Complexity" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{6F0E44E4-9DBC-9E41-B548-48FF281C4DE7}" name="Optimal Complexity" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{4E2B027C-84E2-4746-A050-99003D6F130D}" name=" Brute Force Complexity" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{FBEAA6B8-E7D6-F748-9496-1911EE208A06}" name="Algorithm" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{D488543C-E183-BF44-8C30-17372FA97B14}" name="Data Structure " dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{44ECDE62-26AB-614D-9A95-A825F8E84A50}" name="Progress" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{4426360F-515C-E249-8E56-5FFEBDF610C5}" name="Explanation" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{BDCE3B2A-F2CA-7940-A777-18C5FE8F8250}" name=" Best Complexity" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{6F0E44E4-9DBC-9E41-B548-48FF281C4DE7}" name="Optimal Complexity" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{4E2B027C-84E2-4746-A050-99003D6F130D}" name=" Brute Force Complexity" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1150,15 +1185,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E486DD-8F02-B64F-98E1-BE648EE83720}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="F26" sqref="F2:F26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="27.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="2" customWidth="1"/>
@@ -1645,6 +1680,40 @@
       <c r="G27" s="6"/>
       <c r="H27" s="8"/>
     </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Code review for testing on problem site
</commit_message>
<xml_diff>
--- a/Problems.xlsx
+++ b/Problems.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selman/Google Drive/Master/First Year/First semester/Competitive programming and contests/Github/CompetitiveProgramming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF85CBFE-F2BB-1943-A79F-D571084507CD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C48A24-BBC7-D045-9D1D-281AE5289397}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{59DA6F5E-AF74-844C-9459-D868A740F883}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="50">
   <si>
     <t>Problem</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>Longest Decreasing Subsequence</t>
+  </si>
+  <si>
+    <t>Check on site</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -326,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -361,11 +367,31 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -749,7 +775,6 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr/>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -760,8 +785,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D938C518-70BF-5A4D-B2E3-CBDA392058BE}" name="Table2" displayName="Table2" ref="A1:H30" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H30" xr:uid="{591EFFBC-CF6E-4749-B9B1-AA3DBEFC5570}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D938C518-70BF-5A4D-B2E3-CBDA392058BE}" name="Table2" displayName="Table2" ref="A1:I30" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I30" xr:uid="{591EFFBC-CF6E-4749-B9B1-AA3DBEFC5570}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -770,16 +795,18 @@
     <filterColumn colId="5" hiddenButton="1"/>
     <filterColumn colId="6" hiddenButton="1"/>
     <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{ACAC2441-A820-944F-9AF2-3F5E4FB31EA0}" name="Problem" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{FBEAA6B8-E7D6-F748-9496-1911EE208A06}" name="Algorithm" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{D488543C-E183-BF44-8C30-17372FA97B14}" name="Data Structure " dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{44ECDE62-26AB-614D-9A95-A825F8E84A50}" name="Progress" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{4426360F-515C-E249-8E56-5FFEBDF610C5}" name="Explanation" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{BDCE3B2A-F2CA-7940-A777-18C5FE8F8250}" name=" Best Complexity" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{6F0E44E4-9DBC-9E41-B548-48FF281C4DE7}" name="Optimal Complexity" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{4E2B027C-84E2-4746-A050-99003D6F130D}" name=" Brute Force Complexity" dataDxfId="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{ACAC2441-A820-944F-9AF2-3F5E4FB31EA0}" name="Problem" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{FBEAA6B8-E7D6-F748-9496-1911EE208A06}" name="Algorithm" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{D488543C-E183-BF44-8C30-17372FA97B14}" name="Data Structure " dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{44ECDE62-26AB-614D-9A95-A825F8E84A50}" name="Progress" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{4426360F-515C-E249-8E56-5FFEBDF610C5}" name="Explanation" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{BDCE3B2A-F2CA-7940-A777-18C5FE8F8250}" name=" Best Complexity" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{6F0E44E4-9DBC-9E41-B548-48FF281C4DE7}" name="Optimal Complexity" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{4E2B027C-84E2-4746-A050-99003D6F130D}" name=" Brute Force Complexity" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{1DC48CC5-B051-5142-B7A3-9C876CD94C3C}" name="Check on site" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1082,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E486DD-8F02-B64F-98E1-BE648EE83720}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1101,7 +1128,7 @@
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1126,8 +1153,11 @@
       <c r="H1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -1146,8 +1176,11 @@
       <c r="H2" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
@@ -1168,8 +1201,9 @@
       <c r="H3" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="22"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
@@ -1190,8 +1224,9 @@
       <c r="H4" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="22"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
@@ -1208,8 +1243,9 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
@@ -1232,8 +1268,9 @@
       <c r="H6" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="22"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
@@ -1252,8 +1289,9 @@
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
@@ -1270,8 +1308,9 @@
         <v>33</v>
       </c>
       <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
@@ -1288,8 +1327,9 @@
         <v>33</v>
       </c>
       <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
@@ -1304,8 +1344,9 @@
       <c r="F10" s="3"/>
       <c r="G10" s="6"/>
       <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -1320,8 +1361,9 @@
       <c r="F11" s="3"/>
       <c r="G11" s="6"/>
       <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="22"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
@@ -1336,8 +1378,9 @@
       <c r="F12" s="3"/>
       <c r="G12" s="6"/>
       <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="22"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -1352,8 +1395,9 @@
       <c r="F13" s="3"/>
       <c r="G13" s="6"/>
       <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="22"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
@@ -1368,8 +1412,9 @@
       <c r="F14" s="3"/>
       <c r="G14" s="6"/>
       <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="22"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>14</v>
       </c>
@@ -1384,8 +1429,9 @@
       <c r="F15" s="3"/>
       <c r="G15" s="6"/>
       <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="22"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>16</v>
       </c>
@@ -1400,8 +1446,9 @@
       <c r="F16" s="3"/>
       <c r="G16" s="6"/>
       <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="22"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>17</v>
       </c>
@@ -1416,8 +1463,9 @@
       <c r="F17" s="3"/>
       <c r="G17" s="6"/>
       <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="22"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
@@ -1432,8 +1480,9 @@
       <c r="F18" s="3"/>
       <c r="G18" s="6"/>
       <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="22"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>19</v>
       </c>
@@ -1448,8 +1497,9 @@
       <c r="F19" s="3"/>
       <c r="G19" s="6"/>
       <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="22"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>20</v>
       </c>
@@ -1464,8 +1514,9 @@
       <c r="F20" s="3"/>
       <c r="G20" s="6"/>
       <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="22"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>21</v>
       </c>
@@ -1480,8 +1531,9 @@
       <c r="F21" s="3"/>
       <c r="G21" s="6"/>
       <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="22"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>22</v>
       </c>
@@ -1496,8 +1548,9 @@
       <c r="F22" s="3"/>
       <c r="G22" s="6"/>
       <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="22"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>23</v>
       </c>
@@ -1512,8 +1565,9 @@
       <c r="F23" s="3"/>
       <c r="G23" s="6"/>
       <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="22"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>24</v>
       </c>
@@ -1528,8 +1582,9 @@
       <c r="F24" s="3"/>
       <c r="G24" s="6"/>
       <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="22"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>25</v>
       </c>
@@ -1544,8 +1599,9 @@
       <c r="F25" s="3"/>
       <c r="G25" s="6"/>
       <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="22"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>26</v>
       </c>
@@ -1560,8 +1616,9 @@
       <c r="F26" s="3"/>
       <c r="G26" s="6"/>
       <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="22"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>27</v>
       </c>
@@ -1576,8 +1633,9 @@
       <c r="F27" s="3"/>
       <c r="G27" s="6"/>
       <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="22"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>46</v>
       </c>
@@ -1594,8 +1652,9 @@
       <c r="H28" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="22"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>47</v>
       </c>
@@ -1612,8 +1671,9 @@
       <c r="H29" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="22"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="17"/>
       <c r="C30" s="18"/>
@@ -1622,6 +1682,7 @@
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
       <c r="H30" s="8"/>
+      <c r="I30" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding Binary search to Insertion Sort
</commit_message>
<xml_diff>
--- a/Problems.xlsx
+++ b/Problems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selman/Google Drive/Master/First Year/First semester/Competitive programming and contests/Github/CompetitiveProgramming/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selman/Google Drive/School/Master/First Year/First semester/Competitive programming and contests/Github/CompetitiveProgramming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C48A24-BBC7-D045-9D1D-281AE5289397}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE6381F-956F-4D4F-9B7F-9EFBD9758CAD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{59DA6F5E-AF74-844C-9459-D868A740F883}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{59DA6F5E-AF74-844C-9459-D868A740F883}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
   <si>
     <t>Problem</t>
   </si>
@@ -1111,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E486DD-8F02-B64F-98E1-BE648EE83720}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1125,7 +1125,8 @@
     <col min="6" max="6" width="26" style="2" customWidth="1"/>
     <col min="7" max="7" width="38.1640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="23.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="15.1640625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1201,7 +1202,9 @@
       <c r="H3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="22"/>
+      <c r="I3" s="22" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -1224,7 +1227,9 @@
       <c r="H4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="22"/>
+      <c r="I4" s="22" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
@@ -1243,7 +1248,9 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="22"/>
+      <c r="I5" s="22" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">

</xml_diff>

<commit_message>
Largest Even Number was solved
</commit_message>
<xml_diff>
--- a/Problems.xlsx
+++ b/Problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selman/Google Drive/School/Master/First Year/First semester/Competitive programming and contests/Github/CompetitiveProgramming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE053AD-71B4-624B-9D12-E683E014F36F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3249C0E1-2FA6-4041-82AD-35FD28492ED8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{59DA6F5E-AF74-844C-9459-D868A740F883}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="50">
   <si>
     <t>Problem</t>
   </si>
@@ -174,7 +174,7 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>In Progress</t>
+    <t>O(nlogn)</t>
   </si>
 </sst>
 </file>
@@ -256,7 +256,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,13 +271,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -396,12 +390,12 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1146,7 +1140,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1337,38 +1331,46 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="23" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="22"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
@@ -1402,7 +1404,9 @@
       <c r="F11" s="3"/>
       <c r="G11" s="6"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="22"/>
+      <c r="I11" s="23" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">

</xml_diff>